<commit_message>
combine usekeyword.xlsx & emailtemplate.xlsx into configUBS.xlsx. all settings configure using 1 excel file able to download .pdf files
</commit_message>
<xml_diff>
--- a/Tender/GeBiz_04052021.xlsx
+++ b/Tender/GeBiz_04052021.xlsx
@@ -6,7 +6,8 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Facilities Maintenance" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Library" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Facilities Maintenance" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <x:si>
     <x:t>Reference Number</x:t>
   </x:si>
@@ -47,6 +48,84 @@
   </x:si>
   <x:si>
     <x:t>POC Tel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NLB000ETQ21000035</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invitation to Quote for the Support and Maintenance of Inventorisation System for the National Library Board</x:t>
+  </x:si>
+  <x:si>
+    <x:t>National Library Board</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14 May 2021
+01:00PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invitation to Quote</x:t>
+  </x:si>
+  <x:si>
+    <x:t>no</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LIN YANFEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lin_Yanfen@nlb.gov.sg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NLB000ETQ21000036</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INVITATION TO QUOTE FOR THE PROVISION OF MAINTENANCE SERVICES AND ENHANCEMENTS TO THE WEB ARCHIVE SINGAPORE PORTAL FOR NATIONAL LIBRARY BOARD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHARLES WIJAYA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Charles_Wijaya@nlb.gov.sg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NYP000ETQ21000121</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jointly operate and train students at the Nanyang Polytechnic Library Training Cafe with NYP School of Business Management</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nanyang Polytechnic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 May 2021
+01:00PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 May 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LINDA LIM / PATRICK PNG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>linda_sf_lim@nyp.edu.sg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NLB000ETQ21000030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INVITATION TO QUOTE FOR THE SUPPLY AND DELIVERY OF 55 INCH TOUCHSCREEN WITH PC AND CASTOR WHEELS FOR THE NATIONAL LIBRARY BOARD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>05 May 2021
+01:00PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRIMARYAZMI SAATazmi_saat@nlb.gov.sglayout_RepaintAllLayouts();6704 1099layout_RepaintAllLayouts();layout_RepaintAllLayouts();NLBlayout_RepaintAllLayouts();</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AZMI SAAT</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">JTC000ETT21000013 </x:t>
@@ -65,10 +144,10 @@
     <x:t>Tender</x:t>
   </x:si>
   <x:si>
-    <x:t>no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IVY SIMIvy_SIM@jtc.gov.sglayout_RepaintAllLayouts();6883 3677layout_RepaintAllLayouts();layout_RepaintAllLayouts();The JTC Summit, 8 Jurong Town Hall Road, Singapore 609434layout_RepaintAllLayouts();</x:t>
+    <x:t>10 Mar 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IVY SIM</x:t>
   </x:si>
   <x:si>
     <x:t>Ivy_SIM@jtc.gov.sg</x:t>
@@ -87,10 +166,7 @@
 04:00PM</x:t>
   </x:si>
   <x:si>
-    <x:t>ONG SOH HIANONG_SOH_HIAN@NPARKS.GOV.SGlayout_RepaintAllLayouts();64400046layout_RepaintAllLayouts();layout_RepaintAllLayouts();National Parks Board 
-Headquarters 
-Singapore Botanic Gardens 
-1 Cluny Road, Singapore 259569layout_RepaintAllLayouts();</x:t>
+    <x:t>ONG SOH HIAN</x:t>
   </x:si>
   <x:si>
     <x:t>ONG_SOH_HIAN@NPARKS.GOV.SG</x:t>
@@ -106,12 +182,6 @@
 04:00PM</x:t>
   </x:si>
   <x:si>
-    <x:t>ONG SOH HIANONG_SOH_HIAN@NPARKS.GOV.SGlayout_RepaintAllLayouts();64400046layout_RepaintAllLayouts();layout_RepaintAllLayouts();National Parks Board
-Headquarters
-Singapore Botanic Gardens
-1 Cluny Road, Singapore 259569layout_RepaintAllLayouts();</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">PAR000ETT21000006 </x:t>
   </x:si>
   <x:si>
@@ -121,9 +191,10 @@
     <x:t>Parliament</x:t>
   </x:si>
   <x:si>
-    <x:t>MOHAMMAD AMIN HAMIDMohammad_Amin_HAMID@parl.gov.sglayout_RepaintAllLayouts();6332 6684layout_RepaintAllLayouts();layout_RepaintAllLayouts();Parliament House 
-1 Parliament Place 
-S178880layout_RepaintAllLayouts();</x:t>
+    <x:t>21 Apr 2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MOHAMMAD AMIN HAMID</x:t>
   </x:si>
   <x:si>
     <x:t>Mohammad_Amin_HAMID@parl.gov.sg</x:t>
@@ -140,6 +211,9 @@
   <x:si>
     <x:t>21 May 2021
 04:00PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
   </x:si>
   <x:si>
     <x:t>PRIMARYTAN YUAN HONGTAN_Yuan_Hong@ura.gov.sglayout_RepaintAllLayouts();6321 8213layout_RepaintAllLayouts();layout_RepaintAllLayouts();45 Maxwell Road, The URA Centrelayout_RepaintAllLayouts();</x:t>
@@ -496,6 +570,171 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:K5"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:11">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:11">
+      <x:c r="A2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
+      <x:c r="A3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
+      <x:c r="A4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
+      <x:c r="A5" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:K6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -539,132 +778,150 @@
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>41</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>16</x:v>
+      <x:c r="G5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>56</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>56</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>